<commit_message>
fix some problems wist f str
</commit_message>
<xml_diff>
--- a/hw.xlsx
+++ b/hw.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -143,8 +143,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +266,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -312,7 +320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,9 +352,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,6 +387,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -553,14 +563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
@@ -568,7 +578,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45">
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -579,14 +589,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="45">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -597,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
@@ -608,7 +618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
@@ -619,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -630,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45">
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -641,7 +651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75">
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -652,7 +662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -663,7 +673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>4</v>
       </c>
@@ -674,7 +684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
@@ -685,7 +695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -696,7 +706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>5</v>
       </c>
@@ -707,7 +717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
@@ -718,7 +728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
@@ -729,7 +739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
@@ -740,7 +750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>6</v>
       </c>
@@ -751,7 +761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
@@ -762,7 +772,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>28</v>
       </c>
@@ -773,7 +783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>29</v>
       </c>
@@ -784,7 +794,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>29</v>
       </c>
@@ -795,7 +805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
@@ -806,7 +816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45">
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>35</v>
       </c>
@@ -817,7 +827,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
@@ -828,7 +838,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
@@ -847,14 +857,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="184.5703125" customWidth="1"/>
@@ -866,12 +876,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
add task 6, weather_parse
</commit_message>
<xml_diff>
--- a/hw.xlsx
+++ b/hw.xlsx
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -244,12 +244,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -566,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,10 +701,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -718,10 +712,10 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -729,13 +723,13 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -757,7 +751,7 @@
       <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -790,7 +784,7 @@
       <c r="B20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -801,7 +795,7 @@
       <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="13" t="s">
         <v>33</v>
       </c>
     </row>
@@ -809,10 +803,10 @@
       <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -823,7 +817,7 @@
       <c r="B23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="13" t="s">
         <v>34</v>
       </c>
     </row>
@@ -831,10 +825,10 @@
       <c r="A24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="13" t="s">
         <v>36</v>
       </c>
     </row>
@@ -845,7 +839,7 @@
       <c r="B25" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>